<commit_message>
Finished test case spreadsheet, tester located in test_cases folder in sendApptEmail folder
</commit_message>
<xml_diff>
--- a/test_cases/emailSender_test_cases.xlsx
+++ b/test_cases/emailSender_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anscmc\Desktop\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anscmc\Desktop\Testing\cis315_OfficeHours\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -39,13 +39,124 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Class Tested:</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>EmailSender</t>
+  </si>
+  <si>
+    <t>sendEmailInvite(), setICSEmailValues(), SendEmailWithIcsAttachment()</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Email not sent</t>
+  </si>
+  <si>
+    <t>Emails sent/received with correct information</t>
+  </si>
+  <si>
+    <t>Emails not sent</t>
+  </si>
+  <si>
+    <t>Emails sent and received by both parties, all information was correct</t>
+  </si>
+  <si>
+    <t>Emails not sent, as expected because student email address is NULL</t>
+  </si>
+  <si>
+    <t>Emails not sent, as expected because professor email address is NULL</t>
+  </si>
+  <si>
+    <t>Emails not sent, as expected because student name is NULL</t>
+  </si>
+  <si>
+    <t>Emails not sent, as expected because professor name is NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emails sent </t>
+  </si>
+  <si>
+    <t>Emails sent</t>
+  </si>
+  <si>
+    <t>Message to student was generically created</t>
+  </si>
+  <si>
+    <t>Message to professor was generically created</t>
+  </si>
+  <si>
+    <t>All inputs are NULL, email should not be sent (and cannot without email addresses)</t>
+  </si>
+  <si>
+    <t>Location is NULL, so generic location was created based on professors name as expected</t>
+  </si>
+  <si>
+    <t>Student email is an empty string. Neither email was sent, as expected</t>
+  </si>
+  <si>
+    <t>Student name is an empty string. Should not be accepted by the system</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Professor email an empty string</t>
+  </si>
+  <si>
+    <t>Email sent</t>
+  </si>
+  <si>
+    <t>Should not be accepted by the system, student name is an empty string</t>
+  </si>
+  <si>
+    <t>A generic professor message should be created</t>
+  </si>
+  <si>
+    <t>Student name NULL, system did not accept as expected</t>
+  </si>
+  <si>
+    <t>Professor name NULL, system did not accept as expected</t>
+  </si>
+  <si>
+    <t>Both names NULL, system did not accept as expected</t>
+  </si>
+  <si>
+    <t>Location and email messages are empty strings. Generic placeholders should have been created.</t>
+  </si>
+  <si>
+    <t>Location and email messages are NULL. Generic placeholders were created.</t>
+  </si>
+  <si>
+    <t>Pass/Fail Results:</t>
+  </si>
+  <si>
+    <t>Student message was sent to both parties for unknown reason</t>
+  </si>
+  <si>
+    <t>75% passed, 25% failed</t>
+  </si>
+  <si>
+    <t>Reference:</t>
+  </si>
+  <si>
+    <t>Functions Tested:</t>
+  </si>
+  <si>
+    <t>See test_cases/sendApptEmail for unit testing VS program used for this class.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,16 +164,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -70,11 +195,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -83,7 +279,52 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -106,15 +347,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4565650</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>698500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -144,7 +385,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308100" y="368300"/>
+          <a:off x="1308100" y="317500"/>
           <a:ext cx="4565650" cy="698500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -156,15 +397,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4565650</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>679450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -194,7 +435,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308100" y="1022350"/>
+          <a:off x="1308100" y="1041400"/>
           <a:ext cx="4565650" cy="679450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -206,15 +447,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4565650</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>692150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -244,7 +485,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308100" y="1727200"/>
+          <a:off x="1308100" y="1765300"/>
           <a:ext cx="4565650" cy="692150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -256,15 +497,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4565650</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>679450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -294,7 +535,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="2484783"/>
+          <a:off x="1308100" y="2489200"/>
           <a:ext cx="4565650" cy="679450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -306,15 +547,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4572000</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>704850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -344,7 +585,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="3208130"/>
+          <a:off x="1308100" y="3213100"/>
           <a:ext cx="4572000" cy="704850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -356,15 +597,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1656</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1657</xdr:colOff>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>673100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -394,8 +635,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="3931478"/>
-          <a:ext cx="4584700" cy="673100"/>
+          <a:off x="1308100" y="3937000"/>
+          <a:ext cx="4586356" cy="673100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -406,15 +647,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>3454400</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>692150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -444,7 +685,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="4654826"/>
+          <a:off x="1308100" y="4660900"/>
           <a:ext cx="3454400" cy="692150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -456,15 +697,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>660400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -494,7 +735,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="5378174"/>
+          <a:off x="1308100" y="5384800"/>
           <a:ext cx="1257300" cy="660400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -506,15 +747,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4572000</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>692150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -544,7 +785,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="6101522"/>
+          <a:off x="1308100" y="6108700"/>
           <a:ext cx="4572000" cy="692150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -556,15 +797,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4552950</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>584200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -594,7 +835,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="6824870"/>
+          <a:off x="1308100" y="6832600"/>
           <a:ext cx="4552950" cy="584200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -606,15 +847,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4552950</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>577850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -644,7 +885,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="7548217"/>
+          <a:off x="1308100" y="7556500"/>
           <a:ext cx="4552950" cy="577850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -656,15 +897,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4559300</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>584200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -694,7 +935,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="8271565"/>
+          <a:off x="1308100" y="8280400"/>
           <a:ext cx="4559300" cy="584200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -706,15 +947,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4572000</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>590550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -744,7 +985,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="8994913"/>
+          <a:off x="1308100" y="9004300"/>
           <a:ext cx="4572000" cy="590550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -756,15 +997,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4559300</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>577850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -794,7 +1035,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="9718261"/>
+          <a:off x="1308100" y="9728200"/>
           <a:ext cx="4559300" cy="577850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -806,15 +1047,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>3448050</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>584200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -844,7 +1085,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="10441609"/>
+          <a:off x="1308100" y="10452100"/>
           <a:ext cx="3448050" cy="584200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -856,15 +1097,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4572000</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>590550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -894,7 +1135,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="11164957"/>
+          <a:off x="1308100" y="11176000"/>
           <a:ext cx="4572000" cy="590550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -906,15 +1147,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4559300</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>577850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -944,7 +1185,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="11888304"/>
+          <a:off x="1308100" y="11899900"/>
           <a:ext cx="4559300" cy="577850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -956,15 +1197,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4559300</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>577850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -994,7 +1235,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="12611652"/>
+          <a:off x="1308100" y="12623800"/>
           <a:ext cx="4559300" cy="577850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1006,15 +1247,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>2076450</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>685800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1044,7 +1285,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="13335000"/>
+          <a:off x="1308100" y="13347700"/>
           <a:ext cx="2076450" cy="685800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1056,15 +1297,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>2063750</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>673100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1094,7 +1335,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1308652" y="14058348"/>
+          <a:off x="1308100" y="14071600"/>
           <a:ext cx="2063750" cy="673100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1404,188 +1645,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F23"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.81640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10">
+        <v>42714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E7" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3">
+    <row r="8" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5">
+      <c r="C9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6">
+      <c r="B10" s="2"/>
+      <c r="C10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
         <v>4</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7">
+      <c r="C11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
         <v>5</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8">
+      <c r="C12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
         <v>6</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9">
+      <c r="C13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
         <v>7</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10">
+      <c r="C14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
         <v>8</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11">
+      <c r="C15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12">
+      <c r="E15" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>9</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
         <v>10</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13">
+      <c r="C17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
         <v>11</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14">
+      <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
         <v>12</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15">
+      <c r="C19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
         <v>13</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16">
+      <c r="C20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
         <v>14</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17">
+      <c r="C21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
         <v>15</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18">
+      <c r="C22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
         <v>16</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19">
+      <c r="C23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
         <v>17</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20">
+      <c r="C24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
         <v>18</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21">
+      <c r="C25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
         <v>19</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22">
+      <c r="C26" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
         <v>20</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23">
-        <v>21</v>
+      <c r="C27" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>